<commit_message>
changed around stuff in meat
</commit_message>
<xml_diff>
--- a/food_groups/carbs.xlsx
+++ b/food_groups/carbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C354FD0-1C1B-4758-B14E-59EB8A44BD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463C15C9-EB9A-4A52-81A6-115FF59EF967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carbs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>pass</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>gluten-free pasta</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -434,9 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -449,31 +457,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -481,17 +489,25 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -502,10 +518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CC7064-AEDE-4A62-8A51-F61DE2C2133B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,23 +535,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -543,9 +559,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -556,10 +580,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDE6C27-C7A5-4BCF-A692-68310001891D}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,41 +594,49 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added files to food groups
</commit_message>
<xml_diff>
--- a/food_groups/carbs.xlsx
+++ b/food_groups/carbs.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463C15C9-EB9A-4A52-81A6-115FF59EF967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50512184-F4F5-40F1-BC69-A185C6C529B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carbs" sheetId="1" r:id="rId1"/>
-    <sheet name="potatoes" sheetId="2" r:id="rId2"/>
-    <sheet name="pasta" sheetId="3" r:id="rId3"/>
+    <sheet name="rice" sheetId="5" r:id="rId2"/>
+    <sheet name="potatoes" sheetId="2" r:id="rId3"/>
+    <sheet name="oatmeal" sheetId="9" r:id="rId4"/>
+    <sheet name="grits" sheetId="10" r:id="rId5"/>
+    <sheet name="grain" sheetId="4" r:id="rId6"/>
+    <sheet name="pasta" sheetId="3" r:id="rId7"/>
+    <sheet name="bread" sheetId="6" r:id="rId8"/>
+    <sheet name="white bread" sheetId="7" r:id="rId9"/>
+    <sheet name="wheat bread" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
   <si>
     <t>pass</t>
   </si>
@@ -67,18 +74,12 @@
     <t>potatoes</t>
   </si>
   <si>
-    <t>carbohydrates</t>
-  </si>
-  <si>
     <t>food super group</t>
   </si>
   <si>
     <t>pasta</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>gluten-free substitute</t>
   </si>
   <si>
@@ -89,6 +90,33 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>grain</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>white bread</t>
+  </si>
+  <si>
+    <t>healthy substitute</t>
+  </si>
+  <si>
+    <t>sourdough bread</t>
+  </si>
+  <si>
+    <t>wheat bread</t>
+  </si>
+  <si>
+    <t>oatmeal</t>
+  </si>
+  <si>
+    <t>grits</t>
   </si>
 </sst>
 </file>
@@ -443,7 +471,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,10 +485,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -516,12 +544,118 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9C691C-16B8-4516-9CDE-7AC1C12F3BF6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DA7CD4-CAE2-4CED-898E-81BE54F6B25B}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CC7064-AEDE-4A62-8A51-F61DE2C2133B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,10 +669,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -567,10 +701,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -578,12 +712,177 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B941A56-BB7C-4729-9F12-EC75D373ED68}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D62231-5E1D-46A2-AAEA-872B2B081587}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B692B0-1738-4BDB-AE0E-A4C603A6044F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDE6C27-C7A5-4BCF-A692-68310001891D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,10 +893,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -605,7 +904,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -618,26 +917,128 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1CCF84-B803-486E-A6D4-429C0BA57FD6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A5B1DC-A025-4F41-8FF8-6411B5C6A1A5}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a bunch of csv files, we need to add style description and superclass on these
</commit_message>
<xml_diff>
--- a/food_groups/carbs.xlsx
+++ b/food_groups/carbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50512184-F4F5-40F1-BC69-A185C6C529B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D37EBB-3BEF-40ED-A721-CED20C04782D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carbs" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="grits" sheetId="10" r:id="rId5"/>
     <sheet name="grain" sheetId="4" r:id="rId6"/>
     <sheet name="pasta" sheetId="3" r:id="rId7"/>
-    <sheet name="bread" sheetId="6" r:id="rId8"/>
-    <sheet name="white bread" sheetId="7" r:id="rId9"/>
-    <sheet name="wheat bread" sheetId="8" r:id="rId10"/>
+    <sheet name="noodles" sheetId="11" r:id="rId8"/>
+    <sheet name="bread" sheetId="6" r:id="rId9"/>
+    <sheet name="white bread" sheetId="7" r:id="rId10"/>
+    <sheet name="wheat bread" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="31">
   <si>
     <t>pass</t>
   </si>
@@ -117,6 +118,21 @@
   </si>
   <si>
     <t>grits</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>asian</t>
+  </si>
+  <si>
+    <t>western</t>
+  </si>
+  <si>
+    <t>american</t>
+  </si>
+  <si>
+    <t>noodles</t>
   </si>
 </sst>
 </file>
@@ -468,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,12 +555,79 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A5B1DC-A025-4F41-8FF8-6411B5C6A1A5}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9C691C-16B8-4516-9CDE-7AC1C12F3BF6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -597,10 +680,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DA7CD4-CAE2-4CED-898E-81BE54F6B25B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,6 +728,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -652,10 +743,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CC7064-AEDE-4A62-8A51-F61DE2C2133B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,6 +798,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -714,10 +813,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B941A56-BB7C-4729-9F12-EC75D373ED68}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,6 +865,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -773,10 +880,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D62231-5E1D-46A2-AAEA-872B2B081587}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,6 +932,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -832,10 +947,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B692B0-1738-4BDB-AE0E-A4C603A6044F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,6 +984,14 @@
         <v>7</v>
       </c>
       <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -937,6 +1060,69 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B2055E-AFEE-4140-BD6F-A8C651B8A4F6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1CCF84-B803-486E-A6D4-429C0BA57FD6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -985,63 +1171,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A5B1DC-A025-4F41-8FF8-6411B5C6A1A5}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed typo in excel file
</commit_message>
<xml_diff>
--- a/food_groups/carbs.xlsx
+++ b/food_groups/carbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05FBC98-1547-4D59-86DD-8708E6FA0AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B429025-ED42-409C-9E3E-C6E68D5297A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carbs" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="26">
   <si>
     <t>pass</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>food super group</t>
-  </si>
-  <si>
-    <t>gluten-free substitute</t>
   </si>
   <si>
     <t>property</t>
@@ -527,10 +524,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -583,7 +580,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -591,7 +588,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -606,18 +603,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193F2DC3-3CD9-41BA-B411-7741B292B46A}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -625,7 +625,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,7 +646,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -670,17 +670,20 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -688,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -709,7 +712,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -717,7 +720,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -737,13 +740,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -780,10 +786,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -810,10 +816,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -850,10 +856,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -877,10 +883,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -888,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -917,10 +923,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -944,10 +950,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -955,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -984,10 +990,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1004,13 +1010,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1018,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1039,7 +1048,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1054,18 +1063,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638A66D3-AD9F-4D2A-BEEF-6D27DCC40394}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -1074,7 +1086,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1098,7 +1110,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -1107,7 +1119,7 @@
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -1179,17 +1191,20 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1197,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1218,7 +1233,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1226,10 +1241,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up csv files
</commit_message>
<xml_diff>
--- a/food_groups/carbs.xlsx
+++ b/food_groups/carbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B429025-ED42-409C-9E3E-C6E68D5297A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93545A4-F870-4879-A268-C62FD2E811D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,7 +604,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding extra layer of substitutions
</commit_message>
<xml_diff>
--- a/food_groups/carbs.xlsx
+++ b/food_groups/carbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\NLP-P2\food_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93545A4-F870-4879-A268-C62FD2E811D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C881437D-6DA5-40A3-AC2C-8782DE96AB8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="25">
   <si>
     <t>pass</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>bread</t>
-  </si>
-  <si>
-    <t>food supergroup</t>
   </si>
 </sst>
 </file>
@@ -510,7 +507,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +585,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>

</xml_diff>